<commit_message>
Mark phone numbers and prior balance as optional
</commit_message>
<xml_diff>
--- a/templates/Accounts.xlsx
+++ b/templates/Accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -262,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -293,6 +293,12 @@
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -363,11 +369,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,15 +454,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>25560</xdr:colOff>
+      <xdr:colOff>52200</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -465,8 +471,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="19800"/>
-          <a:ext cx="8589960" cy="8329680"/>
+          <a:off x="54000" y="10800"/>
+          <a:ext cx="6598800" cy="8329320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -489,6 +495,9 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:uFill>
                 <a:solidFill>
                   <a:srgbClr val="ffffff"/>
@@ -506,6 +515,9 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:uFill>
                 <a:solidFill>
                   <a:srgbClr val="ffffff"/>
@@ -523,6 +535,9 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:uFill>
                 <a:solidFill>
                   <a:srgbClr val="ffffff"/>
@@ -666,11 +681,14 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T26" activeCellId="0" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -692,36 +710,38 @@
   </sheetPr>
   <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA9" activeCellId="0" sqref="AA9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.1683673469388"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,22 +805,22 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AMJ1" s="0"/>

</xml_diff>

<commit_message>
Double quoted strings are not required
</commit_message>
<xml_diff>
--- a/templates/Accounts.xlsx
+++ b/templates/Accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -286,6 +286,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -293,12 +299,6 @@
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -454,15 +454,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>52200</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -471,8 +471,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="10800"/>
-          <a:ext cx="6598800" cy="8329320"/>
+          <a:off x="81000" y="1800"/>
+          <a:ext cx="6493680" cy="8328960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -643,26 +643,6 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>All strings should be wrapped in double quotes (e.g. “Simon Westlake”)</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
             <a:t>Within the data sheet, columns with a blue header are optional. Columns with a grey header are required.</a:t>
           </a:r>
           <a:endParaRPr/>
@@ -681,13 +661,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T26" activeCellId="0" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -710,38 +690,38 @@
   </sheetPr>
   <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Moving balance importing to the existing standalone function.
</commit_message>
<xml_diff>
--- a/templates/Accounts.xlsx
+++ b/templates/Accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -35,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>An available ID to use for the account identifier. This must be a number, and it must be unique and currently unused.</t>
+          <t xml:space="preserve">An available ID to use for the account identifier. This must be a number, and it must be unique and currently unused.</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This must be a valid account type ID. Valid built in IDs are 1 for residential and 2 for commercial.</t>
+          <t xml:space="preserve">This must be a valid account type ID. Valid built in IDs are 1 for residential and 2 for commercial.</t>
         </r>
       </text>
     </comment>
@@ -61,7 +61,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This must be a valid account status ID. Built in IDs are 1 for lead, 2 for active and 3 for inactive.</t>
+          <t xml:space="preserve">This must be a valid account status ID. Built in IDs are 1 for lead, 2 for active and 3 for inactive.</t>
         </r>
       </text>
     </comment>
@@ -74,7 +74,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>If you wish to place this account in any groups, add a comma separated list of group IDs here.</t>
+          <t xml:space="preserve">If you wish to place this account in any groups, add a comma separated list of group IDs here.</t>
         </r>
       </text>
     </comment>
@@ -87,7 +87,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>If this account should have sub accounts, add a comma separated list of account IDs here. The sub accounts must exist prior to this account being created, so the order in this document is important.</t>
+          <t xml:space="preserve">If this account should have sub accounts, add a comma separated list of account IDs here. The sub accounts must exist prior to this account being created, so the order in this document is important.</t>
         </r>
       </text>
     </comment>
@@ -100,7 +100,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This is optional, and should only be set if needed. The format is YYYY-MM-DD e.g. 2016-01-01, and the 'day' portion of the bill date must match the accounts 'Bill Day' parameter.</t>
+          <t xml:space="preserve">This is optional, and should only be set if needed. The format is YYYY-MM-DD e.g. 2016-01-01, and the 'day' portion of the bill date must match the accounts 'Bill Day' parameter.</t>
         </r>
       </text>
     </comment>
@@ -113,7 +113,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>County can be excluded as long as the address properly geocodes. The county must be selected from the list of counties available in Sonar via the API and is only used for addresses in the USA. If this is a US address, it is recommended that you enter it validly and exclude the country – the Sonar importer will attempt to determine it automatically.</t>
+          <t xml:space="preserve">County can be excluded as long as the address properly geocodes. The county must be selected from the list of counties available in Sonar via the API and is only used for addresses in the USA. If this is a US address, it is recommended that you enter it validly and exclude the country – the Sonar importer will attempt to determine it automatically.</t>
         </r>
       </text>
     </comment>
@@ -126,7 +126,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This must be a valid 2 character country code from https://en.wikipedia.org/wiki/ISO_3166-1_alpha-2</t>
+          <t xml:space="preserve">This must be a valid 2 character country code from https://en.wikipedia.org/wiki/ISO_3166-1_alpha-2</t>
         </r>
       </text>
     </comment>
@@ -139,7 +139,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Latitude and longitude can be excluded as long as the address properly geocodes.
+          <t xml:space="preserve">Latitude and longitude can be excluded as long as the address properly geocodes.
 </t>
         </r>
       </text>
@@ -153,20 +153,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>A list of the email message categories for the primary contact, separated by a comma. Valid IDs are 2 for financial, 3 for general, 4 for services and 5 for outage notification. If you want the contact to receive all emails, enter 2,3,4,5</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>This should be entered as a number, no currency symbol. Enter a negative number if the customer is owed services (e.g. they overpaid) and a positive number if they have an unpaid balance. Leave blank or enter '0' if you do not wish to import a prior balance.</t>
+          <t xml:space="preserve">A list of the email message categories for the primary contact, separated by a comma. Valid IDs are 2 for financial, 3 for general, 4 for services and 5 for outage notification. If you want the contact to receive all emails, enter 2,3,4,5</t>
         </r>
       </text>
     </comment>
@@ -175,84 +162,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Account Type ID</t>
-  </si>
-  <si>
-    <t>Account Status ID</t>
-  </si>
-  <si>
-    <t>Account Groups</t>
-  </si>
-  <si>
-    <t>Sub Accounts</t>
-  </si>
-  <si>
-    <t>Next Bill Date</t>
-  </si>
-  <si>
-    <t>Physical Address Line1</t>
-  </si>
-  <si>
-    <t>Physical Address Line 2</t>
-  </si>
-  <si>
-    <t>Physical City</t>
-  </si>
-  <si>
-    <t>Physical State</t>
-  </si>
-  <si>
-    <t>Physical County</t>
-  </si>
-  <si>
-    <t>Physical ZIP</t>
-  </si>
-  <si>
-    <t>Physical Country</t>
-  </si>
-  <si>
-    <t>Physical Latitude</t>
-  </si>
-  <si>
-    <t>Physical Longitude</t>
-  </si>
-  <si>
-    <t>Primary Contact Name</t>
-  </si>
-  <si>
-    <t>Primary Contact Role</t>
-  </si>
-  <si>
-    <t>Primary Contact Email Address</t>
-  </si>
-  <si>
-    <t>Primary Contact Email Message Categories</t>
-  </si>
-  <si>
-    <t>Work Phone</t>
-  </si>
-  <si>
-    <t>Work Extension</t>
-  </si>
-  <si>
-    <t>Home Phone</t>
-  </si>
-  <si>
-    <t>Mobile Phone</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t>Prior Balance</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Type ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Status ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next Bill Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Address Line1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Address Line 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical County</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical ZIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Contact Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Contact Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Contact Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Contact Email Message Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fax</t>
   </si>
 </sst>
 </file>
@@ -260,7 +244,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -288,19 +272,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -460,9 +444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>78840</xdr:colOff>
+      <xdr:colOff>78480</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -472,7 +456,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="1800"/>
-          <a:ext cx="6493680" cy="8328960"/>
+          <a:ext cx="6388560" cy="8328600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,7 +478,7 @@
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -507,14 +491,34 @@
             </a:rPr>
             <a:t>This template is to be used for account imports.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -527,14 +531,34 @@
             </a:rPr>
             <a:t>One critical part of this template is the address handling. Sonar requires accurate, specifically formatted addresses in order to properly apply taxation. All addresses entered will be run through the Sonar validator, which may result in some reformatting.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -548,7 +572,7 @@
             <a:t>If an address cannot be validated, as long as the individual fields can be validated, the address will still be entered. If you need to test validation of an address, try to enter it at </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike" u="sng">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike" u="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -563,7 +587,7 @@
             <a:t>https://maps.bing.com</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -576,14 +600,34 @@
             </a:rPr>
             <a:t>. If it is not found, then it is likely that the Sonar validator will fail and you will have to be especially careful to format it in a way that Sonar will understand.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -597,7 +641,7 @@
             <a:t>If you have questions about the formatting of addresses, please check with Sonar support (</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike" u="sng">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike" u="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -612,7 +656,7 @@
             <a:t>support@sonar.software</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -625,14 +669,34 @@
             </a:rPr>
             <a:t>) before proceeding.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -645,7 +709,17 @@
             </a:rPr>
             <a:t>Within the data sheet, columns with a blue header are optional. Columns with a grey header are required.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -667,7 +741,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -690,38 +764,36 @@
   </sheetPr>
   <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,9 +872,7 @@
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
   </sheetData>

</xml_diff>